<commit_message>
Redundent revisions of inferior work
</commit_message>
<xml_diff>
--- a/Formal_Lab_Tom/Formal_Data.xlsx
+++ b/Formal_Lab_Tom/Formal_Data.xlsx
@@ -22,6 +22,7 @@
     <definedName name="wing_area">Sheet1!$C$8</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -167,14 +168,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,134 +483,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1.2889999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>2.5790000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f>Rc_/Ct</f>
         <v>2.0007757951900702</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f>(Rc_/28)*30</f>
         <v>2.7632142857142856</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f>0.5*(Cchord+Ct)*bspan</f>
         <v>121.56642857142856</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <f>bspan^2/wing_area</f>
         <v>29.613438860587689</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>1.75</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f>(Ttc+Trc)*2.75</f>
         <v>7.5625</v>
       </c>

</xml_diff>